<commit_message>
Added testcases for C3DC phs00468
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC04_C3DC_phs000471_AnatomicSite-C649KidneyNOS.xlsx
+++ b/InputFiles/C3DC/TC04_C3DC_phs000471_AnatomicSite-C649KidneyNOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676F0AF5-14D0-C547-A939-AAD5ABC314F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C86A71D-F5C5-5E44-8BFA-B918B86F38F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -146,43 +146,6 @@
 LIMIT 100;</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-    prt.participant_id AS "Participant Id",
-    dgn.diagnosis_id AS "Diagnosis Id",
-    dgn.diagnosis AS "Diagnosis",
-    dgn.diagnosis_classification_system AS "Diagnosis Classification System",
-    dgn.diagnosis_basis AS "Diagnosis Basis",
-    dgn.tumor_classification AS "Tumor Classification",
-    dgn.anatomic_site AS "Anatomic Site",
-    CASE 
-    WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
-    WHEN dgn.age_at_diagnosis &gt;= 1000 THEN 
-        substr(dgn.age_at_diagnosis, 1, length(dgn.age_at_diagnosis) - 3) || ',' || substr(dgn.age_at_diagnosis, -3)
-    ELSE 
-        dgn.age_at_diagnosis 
-END AS "Age at Diagnosis (days)",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000471' AND dgn.anatomic_site = 'C64.9 : Kidney, NOS' AND dgn.diagnosis_id IS NOT NULL
-ORDER BY 
-    prt.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SELECT
     DISTINCT prt.participant_id AS "Participant Id",
     trt.treatment_id AS "Treatment Id",
@@ -293,14 +256,58 @@
     prt.participant_id ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    dgn.diagnosis_id AS "Diagnosis Id",
+    dgn.diagnosis AS "Diagnosis",
+    dgn.diagnosis_classification_system AS "Diagnosis Classification System",
+    dgn.diagnosis_basis AS "Diagnosis Basis",
+    dgn.tumor_classification AS "Tumor Classification",
+    dgn.anatomic_site AS "Anatomic Site",
+    CASE 
+    WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
+    WHEN dgn.age_at_diagnosis &gt;= 1000 THEN 
+        substr(dgn.age_at_diagnosis, 1, length(dgn.age_at_diagnosis) - 3) || ',' || substr(dgn.age_at_diagnosis, -3)
+    ELSE 
+        dgn.age_at_diagnosis 
+END AS "Age at Diagnosis (days)",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs000471' AND dgn.anatomic_site = 'C64.9 : Kidney, NOS' AND dgn.diagnosis_id IS NOT NULL
+ORDER BY 
+    dgn.diagnosis_id ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -353,11 +360,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -683,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,8 +752,8 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -752,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -761,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -770,7 +780,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -782,7 +792,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated C3DC phs000471 testcases
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC04_C3DC_phs000471_AnatomicSite-C649KidneyNOS.xlsx
+++ b/InputFiles/C3DC/TC04_C3DC_phs000471_AnatomicSite-C649KidneyNOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C86A71D-F5C5-5E44-8BFA-B918B86F38F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55F6DC2-6564-A944-B005-AF316650144D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -224,41 +224,6 @@
   <si>
     <t>SELECT DISTINCT
     prt.participant_id AS "Participant Id",
-    srv.survival_id AS "Survival Id",
-    srv.last_known_survival_status AS "Last Known Survival Status",
-    CASE 
-    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
-    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
-        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
-    ELSE 
-        srv.age_at_last_known_survival_status 
-END AS "Age at Last Known Survival Status",
-    srv.first_event AS "First Event",
-    srv.cause_of_death AS "Cause of Death",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000471' AND dgn.anatomic_site = 'C64.9 : Kidney, NOS' AND srv.survival_id IS NOT NULL
-ORDER BY 
-    prt.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    prt.participant_id AS "Participant Id",
     dgn.diagnosis_id AS "Diagnosis Id",
     dgn.diagnosis AS "Diagnosis",
     dgn.diagnosis_classification_system AS "Diagnosis Classification System",
@@ -293,14 +258,56 @@
     dgn.diagnosis_id ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    srv.survival_id AS "Survival Id",
+    srv.last_known_survival_status AS "Last Known Survival Status",
+    CASE 
+    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
+    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
+        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
+    ELSE 
+        srv.age_at_last_known_survival_status 
+END AS "Age at Last Known Survival Status",
+    srv.first_event AS "First Event",
+    srv.cause_of_death AS "Cause of Death",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs000471' AND dgn.anatomic_site = 'C64.9 : Kidney, NOS' AND srv.survival_id IS NOT NULL
+ORDER BY 
+    srv.survival_id ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -360,11 +367,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -779,8 +789,8 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -792,7 +802,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>